<commit_message>
new data and 止损期望
</commit_message>
<xml_diff>
--- a/波动费用占比.xlsx
+++ b/波动费用占比.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="费用占比" sheetId="1" r:id="rId1"/>
     <sheet name="50日ATR" sheetId="3" r:id="rId2"/>
+    <sheet name="50ATRma看整k" sheetId="5" r:id="rId3"/>
+    <sheet name="5050概率" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="546">
   <si>
     <t>费用形式</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1548,29 +1550,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>菜油</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>OI</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>一手保证金</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1618,6 +1597,497 @@
   <si>
     <t>平今3倍</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>菜油</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>OI</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续次数</t>
+  </si>
+  <si>
+    <t>出现的次数</t>
+  </si>
+  <si>
+    <t>百分比</t>
+  </si>
+  <si>
+    <t>累积和</t>
+  </si>
+  <si>
+    <t>看C列，每个都是上一个的一半概率</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>连续</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>次同向的概率是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3.15%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>次内转向的概率</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>96.87%</t>
+    </r>
+  </si>
+  <si>
+    <t>count  895.000000  895.000000  895.000000</t>
+  </si>
+  <si>
+    <t>mean     0.061900    0.542322   -0.469705</t>
+  </si>
+  <si>
+    <t>std      0.810721    0.617726    0.575324</t>
+  </si>
+  <si>
+    <t>25%     -0.334916    0.175761   -0.656740</t>
+  </si>
+  <si>
+    <t>50%      0.023267    0.391389   -0.339723</t>
+  </si>
+  <si>
+    <t>75%      0.446059    0.747572   -0.127285</t>
+  </si>
+  <si>
+    <t>max      4.841334    4.919460    2.664768</t>
+  </si>
+  <si>
+    <t>count  1811.000000  1811.000000  1811.000000</t>
+  </si>
+  <si>
+    <t>mean      0.078891     0.563906    -0.432590</t>
+  </si>
+  <si>
+    <t>std       0.888201     0.747160     0.676665</t>
+  </si>
+  <si>
+    <t>25%      -0.428894     0.124883    -0.752389</t>
+  </si>
+  <si>
+    <t>50%       0.020300     0.438982    -0.362194</t>
+  </si>
+  <si>
+    <t>75%       0.544743     0.890920    -0.062263</t>
+  </si>
+  <si>
+    <t>max       4.705103     4.870775     3.418803</t>
+  </si>
+  <si>
+    <t>对比例</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>count  1917.000000  1917.000000  1917.000000</t>
+  </si>
+  <si>
+    <t>mean      0.052769     0.544121    -0.423313</t>
+  </si>
+  <si>
+    <t>std       0.833310     0.721763     0.669045</t>
+  </si>
+  <si>
+    <t>min      -3.240059    -3.019146    -5.227882</t>
+  </si>
+  <si>
+    <t>25%      -0.398010     0.135501    -0.704225</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.417910    -0.352977</t>
+  </si>
+  <si>
+    <t>75%       0.448096     0.820051    -0.073565</t>
+  </si>
+  <si>
+    <t>count  1152.000000  1152.000000  1152.000000</t>
+  </si>
+  <si>
+    <t>mean      0.036963     0.535544    -0.463287</t>
+  </si>
+  <si>
+    <t>std       0.816024     0.658249     0.595685</t>
+  </si>
+  <si>
+    <t>25%      -0.403629     0.147886    -0.714784</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.388396    -0.382518</t>
+  </si>
+  <si>
+    <t>75%       0.416456     0.787503    -0.120813</t>
+  </si>
+  <si>
+    <t>max       3.526711     4.733728     2.984140</t>
+  </si>
+  <si>
+    <t>count  1079.000000  1079.000000  1079.000000</t>
+  </si>
+  <si>
+    <t>mean      0.050770     0.563628    -0.443977</t>
+  </si>
+  <si>
+    <t>std       0.791261     0.610059     0.602373</t>
+  </si>
+  <si>
+    <t>25%      -0.380364     0.197158    -0.676902</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.437227    -0.343446</t>
+  </si>
+  <si>
+    <t>75%       0.465414     0.837890    -0.115673</t>
+  </si>
+  <si>
+    <t>count  1224.000000  1224.000000  1224.000000</t>
+  </si>
+  <si>
+    <t>mean      0.034345     0.527819    -0.459847</t>
+  </si>
+  <si>
+    <t>std       0.856148     0.698009     0.666119</t>
+  </si>
+  <si>
+    <t>min      -3.250000    -1.689528    -3.724285</t>
+  </si>
+  <si>
+    <t>25%      -0.474668     0.105580    -0.771351</t>
+  </si>
+  <si>
+    <t>50%       0.004055     0.435415    -0.387253</t>
+  </si>
+  <si>
+    <t>75%       0.496735     0.856178    -0.065740</t>
+  </si>
+  <si>
+    <t>max       3.797170     3.915094     3.040973</t>
+  </si>
+  <si>
+    <t>count  1166.000000  1166.000000  1166.000000</t>
+  </si>
+  <si>
+    <t>mean     -0.016721     0.404033    -0.418576</t>
+  </si>
+  <si>
+    <t>std       0.714391     0.541990     0.609616</t>
+  </si>
+  <si>
+    <t>25%      -0.396818     0.129034    -0.708460</t>
+  </si>
+  <si>
+    <t>50%       0.025536     0.379701    -0.325025</t>
+  </si>
+  <si>
+    <t>75%       0.437273     0.684933    -0.026608</t>
+  </si>
+  <si>
+    <t>count  1114.000000  1114.000000  1114.000000</t>
+  </si>
+  <si>
+    <t>mean     -0.064622     0.409800    -0.496728</t>
+  </si>
+  <si>
+    <t>std       0.741831     0.552593     0.628010</t>
+  </si>
+  <si>
+    <t>25%      -0.424648     0.120018    -0.748491</t>
+  </si>
+  <si>
+    <t>50%       0.004347     0.369459    -0.366628</t>
+  </si>
+  <si>
+    <t>75%       0.322451     0.648390    -0.091470</t>
+  </si>
+  <si>
+    <t>max       2.646986     2.914798     1.262417</t>
+  </si>
+  <si>
+    <t>count  1238.000000  1238.000000  1238.000000</t>
+  </si>
+  <si>
+    <t>mean     -0.019051     0.431948    -0.472596</t>
+  </si>
+  <si>
+    <t>std       0.725833     0.533333     0.558147</t>
+  </si>
+  <si>
+    <t>25%      -0.426550     0.113737    -0.755551</t>
+  </si>
+  <si>
+    <t>50%       0.020635     0.349902    -0.354862</t>
+  </si>
+  <si>
+    <t>75%       0.382947     0.658877    -0.114484</t>
+  </si>
+  <si>
+    <t>count  1742.000000  1742.000000  1742.000000</t>
+  </si>
+  <si>
+    <t>mean     -0.002464     0.414583    -0.438494</t>
+  </si>
+  <si>
+    <t>std       0.747565     0.568241     0.629288</t>
+  </si>
+  <si>
+    <t>25%      -0.348866     0.106809    -0.672635</t>
+  </si>
+  <si>
+    <t>50%       0.017885     0.360828    -0.332626</t>
+  </si>
+  <si>
+    <t>75%       0.380796     0.669813    -0.078125</t>
+  </si>
+  <si>
+    <t>max       3.074866     3.275401     2.043400</t>
+  </si>
+  <si>
+    <t>count  914.000000  914.000000  914.000000</t>
+  </si>
+  <si>
+    <t>mean    -0.095994    0.437899   -0.571016</t>
+  </si>
+  <si>
+    <t>std      0.785264    0.506566    0.616828</t>
+  </si>
+  <si>
+    <t>min     -3.752469   -1.722301   -4.502237</t>
+  </si>
+  <si>
+    <t>25%     -0.487723    0.132981   -0.776329</t>
+  </si>
+  <si>
+    <t>50%     -0.059207    0.371242   -0.421496</t>
+  </si>
+  <si>
+    <t>75%      0.348172    0.646771   -0.184263</t>
+  </si>
+  <si>
+    <t>max      3.071581    4.139957    0.696180</t>
+  </si>
+  <si>
+    <t>ma20上</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>看整体没多少优势</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>看整k</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>看收盘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MA向后置换5天</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>count  1090.000000  1090.000000  1090.000000</t>
+  </si>
+  <si>
+    <t>mean      0.053620     0.526722    -0.463680</t>
+  </si>
+  <si>
+    <t>std       0.787494     0.589640     0.551717</t>
+  </si>
+  <si>
+    <t>25%      -0.342013     0.175151    -0.660914</t>
+  </si>
+  <si>
+    <t>50%       0.025250     0.381132    -0.338486</t>
+  </si>
+  <si>
+    <t>75%       0.452654     0.735514    -0.133016</t>
+  </si>
+  <si>
+    <t>count  2170.000000  2170.000000  2170.000000</t>
+  </si>
+  <si>
+    <t>mean      0.063192     0.546821    -0.431842</t>
+  </si>
+  <si>
+    <t>std       0.865565     0.766083     0.667763</t>
+  </si>
+  <si>
+    <t>25%      -0.429093     0.117257    -0.757748</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.422273    -0.371149</t>
+  </si>
+  <si>
+    <t>75%       0.515907     0.857209    -0.058661</t>
+  </si>
+  <si>
+    <t>count  1425.000000  1425.000000  1425.000000</t>
+  </si>
+  <si>
+    <t>mean      0.039910     0.531231    -0.459469</t>
+  </si>
+  <si>
+    <t>std       0.803241     0.645424     0.579518</t>
+  </si>
+  <si>
+    <t>25%      -0.383877     0.157081    -0.713575</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.391061    -0.379957</t>
+  </si>
+  <si>
+    <t>75%       0.416171     0.785482    -0.121310</t>
+  </si>
+  <si>
+    <t>count  1344.000000  1344.000000  1344.000000</t>
+  </si>
+  <si>
+    <t>mean      0.042981     0.553743    -0.441139</t>
+  </si>
+  <si>
+    <t>std       0.772080     0.595819     0.584085</t>
+  </si>
+  <si>
+    <t>25%      -0.385645     0.195748    -0.682341</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.428276    -0.351088</t>
+  </si>
+  <si>
+    <t>75%       0.438773     0.814763    -0.103356</t>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>count  1752.000000  1752.000000  1752.000000</t>
+  </si>
+  <si>
+    <t>mean      0.057541     0.553826    -0.439836</t>
+  </si>
+  <si>
+    <t>std       0.785661     0.663574     0.587329</t>
+  </si>
+  <si>
+    <t>min      -4.443054    -1.696429    -7.281553</t>
+  </si>
+  <si>
+    <t>25%      -0.353904     0.174572    -0.652604</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.423430    -0.353649</t>
+  </si>
+  <si>
+    <t>75%       0.400178     0.773004    -0.129372</t>
+  </si>
+  <si>
+    <t>max       6.039604     7.227723     3.875969</t>
+  </si>
+  <si>
+    <t>mean     -0.023943     0.436236    -0.472182</t>
+  </si>
+  <si>
+    <t>std       0.728579     0.560517     0.603518</t>
+  </si>
+  <si>
+    <t>min      -4.874835    -4.597107    -4.874835</t>
+  </si>
+  <si>
+    <t>25%      -0.402253     0.130208    -0.678295</t>
+  </si>
+  <si>
+    <t>50%       0.000000     0.368732    -0.367647</t>
+  </si>
+  <si>
+    <t>75%       0.364299     0.622172    -0.124792</t>
+  </si>
+  <si>
+    <t>max       3.793467     4.477612     2.823920</t>
   </si>
 </sst>
 </file>
@@ -1790,14 +2260,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -1806,6 +2268,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1901,7 +2368,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1932,19 +2399,23 @@
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="4" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="4" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -2248,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2272,7 +2743,7 @@
         <v>2</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>6</v>
@@ -2343,7 +2814,7 @@
         <v>403</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>391</v>
@@ -2373,9 +2844,9 @@
         <v>369</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="F9" s="31" t="s">
+        <v>407</v>
+      </c>
+      <c r="F9" s="30" t="s">
         <v>370</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -2393,17 +2864,17 @@
       <c r="K9" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="L9" s="32" t="s">
-        <v>415</v>
-      </c>
-      <c r="M9" s="29" t="s">
-        <v>410</v>
+      <c r="L9" s="31" t="s">
+        <v>414</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>409</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="31" t="s">
-        <v>416</v>
+      <c r="O9" s="30" t="s">
+        <v>415</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>1</v>
@@ -2413,7 +2884,7 @@
       <c r="A10" s="17" t="s">
         <v>388</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>400.9</v>
       </c>
       <c r="C10" s="17">
@@ -2422,44 +2893,44 @@
       <c r="D10" s="17">
         <v>5</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="34">
         <f>C10*D10*0.08</f>
         <v>9218</v>
       </c>
-      <c r="F10" s="35">
-        <f>B10*D10</f>
+      <c r="F10" s="34">
+        <f t="shared" ref="F10:F34" si="0">B10*D10</f>
         <v>2004.5</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <v>3.6</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="27">
         <v>1.8</v>
       </c>
       <c r="J10" s="17">
         <v>5</v>
       </c>
       <c r="K10" s="17">
-        <f>(D10*J10)</f>
+        <f t="shared" ref="K10:K34" si="1">(D10*J10)</f>
         <v>25</v>
       </c>
-      <c r="L10" s="20">
-        <f>F10/(H10+I10)</f>
+      <c r="L10" s="17">
+        <f t="shared" ref="L10:L34" si="2">F10/(H10+I10)</f>
         <v>371.2037037037037</v>
       </c>
-      <c r="M10" s="26">
-        <f>B10/C10</f>
+      <c r="M10" s="25">
+        <f t="shared" ref="M10:M34" si="3">B10/C10</f>
         <v>1.7396398351052288E-2</v>
       </c>
       <c r="N10" s="17">
-        <f>F10/K10</f>
+        <f t="shared" ref="N10:N34" si="4">F10/K10</f>
         <v>80.180000000000007</v>
       </c>
-      <c r="O10" s="24">
-        <f>F10/E10</f>
+      <c r="O10" s="25">
+        <f t="shared" ref="O10:O34" si="5">F10/E10</f>
         <v>0.21745497938815361</v>
       </c>
       <c r="P10" s="5" t="s">
@@ -2470,7 +2941,7 @@
       <c r="A11" s="17" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="27">
         <v>1915.8</v>
       </c>
       <c r="C11" s="17">
@@ -2479,44 +2950,44 @@
       <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="34">
         <f>C11*D11*0.07</f>
         <v>10154.200000000001</v>
       </c>
-      <c r="F11" s="35">
-        <f>B11*D11</f>
+      <c r="F11" s="34">
+        <f t="shared" si="0"/>
         <v>1915.8</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <v>3.6</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="27">
         <v>1.8</v>
       </c>
       <c r="J11" s="17">
         <v>10</v>
       </c>
       <c r="K11" s="17">
-        <f>(D11*J11)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L11" s="20">
-        <f>F11/(H11+I11)</f>
+      <c r="L11" s="17">
+        <f t="shared" si="2"/>
         <v>354.77777777777777</v>
       </c>
-      <c r="M11" s="26">
-        <f>B11/C11</f>
+      <c r="M11" s="25">
+        <f t="shared" si="3"/>
         <v>1.320694884875224E-2</v>
       </c>
       <c r="N11" s="17">
-        <f>F11/K11</f>
+        <f t="shared" si="4"/>
         <v>191.57999999999998</v>
       </c>
-      <c r="O11" s="26">
-        <f>F11/E11</f>
+      <c r="O11" s="25">
+        <f t="shared" si="5"/>
         <v>0.1886706978393177</v>
       </c>
       <c r="P11" s="5" t="s">
@@ -2524,10 +2995,10 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="20" t="s">
-        <v>407</v>
-      </c>
-      <c r="B12" s="28">
+      <c r="A12" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="27">
         <v>103.7</v>
       </c>
       <c r="C12" s="17">
@@ -2540,40 +3011,40 @@
         <f>C12*D12*0.07</f>
         <v>4558.4000000000005</v>
       </c>
-      <c r="F12" s="17">
-        <f>B12*D12</f>
+      <c r="F12" s="34">
+        <f t="shared" si="0"/>
         <v>1037</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>2.4</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <v>1.2</v>
       </c>
       <c r="J12" s="17">
         <v>1</v>
       </c>
       <c r="K12" s="17">
-        <f>(D12*J12)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L12" s="20">
-        <f>F12/(H12+I12)</f>
+      <c r="L12" s="17">
+        <f t="shared" si="2"/>
         <v>288.0555555555556</v>
       </c>
-      <c r="M12" s="26">
-        <f>B12/C12</f>
+      <c r="M12" s="25">
+        <f t="shared" si="3"/>
         <v>1.5924447174447173E-2</v>
       </c>
       <c r="N12" s="17">
-        <f>F12/K12</f>
+        <f t="shared" si="4"/>
         <v>103.7</v>
       </c>
-      <c r="O12" s="24">
-        <f>F12/E12</f>
+      <c r="O12" s="25">
+        <f t="shared" si="5"/>
         <v>0.22749210249210247</v>
       </c>
       <c r="P12" s="5" t="s">
@@ -2584,7 +3055,7 @@
       <c r="A13" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>62.34</v>
       </c>
       <c r="C13" s="17">
@@ -2598,47 +3069,47 @@
         <v>2366</v>
       </c>
       <c r="F13" s="17">
-        <f>B13*D13</f>
+        <f t="shared" si="0"/>
         <v>623.40000000000009</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>1.2</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="27">
         <v>1.2</v>
       </c>
       <c r="J13" s="17">
         <v>1</v>
       </c>
       <c r="K13" s="17">
-        <f>(D13*J13)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L13" s="20">
-        <f>F13/(H13+I13)</f>
+      <c r="L13" s="17">
+        <f t="shared" si="2"/>
         <v>259.75000000000006</v>
       </c>
       <c r="M13" s="23">
-        <f>B13/C13</f>
+        <f t="shared" si="3"/>
         <v>1.8443786982248522E-2</v>
       </c>
       <c r="N13" s="17">
-        <f>F13/K13</f>
+        <f t="shared" si="4"/>
         <v>62.340000000000011</v>
       </c>
-      <c r="O13" s="24">
-        <f>F13/E13</f>
+      <c r="O13" s="25">
+        <f t="shared" si="5"/>
         <v>0.26348267117497892</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="25" customFormat="1">
+    <row r="14" spans="1:16" s="24" customFormat="1">
       <c r="A14" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="27">
         <v>290.3</v>
       </c>
       <c r="C14" s="17">
@@ -2647,55 +3118,55 @@
       <c r="D14" s="17">
         <v>10</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="34">
         <f>C14*D14*0.09</f>
         <v>9508.5</v>
       </c>
-      <c r="F14" s="35">
-        <f>B14*D14</f>
+      <c r="F14" s="34">
+        <f t="shared" si="0"/>
         <v>2903</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <f>C14*D14*0.000054</f>
         <v>5.7050999999999998</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="27">
         <f>C14*D14*0.000054</f>
         <v>5.7050999999999998</v>
       </c>
       <c r="J14" s="17">
         <v>5</v>
       </c>
-      <c r="K14" s="17">
-        <f>(D14*J14)</f>
+      <c r="K14" s="34">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="L14" s="20">
-        <f>F14/(H14+I14)</f>
+      <c r="L14" s="17">
+        <f t="shared" si="2"/>
         <v>254.42148253317208</v>
       </c>
       <c r="M14" s="16">
-        <f>B14/C14</f>
+        <f t="shared" si="3"/>
         <v>2.7477520113582586E-2</v>
       </c>
       <c r="N14" s="17">
-        <f>F14/K14</f>
+        <f t="shared" si="4"/>
         <v>58.06</v>
       </c>
-      <c r="O14" s="24">
-        <f>F14/E14</f>
+      <c r="O14" s="25">
+        <f t="shared" si="5"/>
         <v>0.30530577903980649</v>
       </c>
       <c r="P14"/>
     </row>
-    <row r="15" spans="1:16" s="25" customFormat="1">
+    <row r="15" spans="1:16" s="24" customFormat="1">
       <c r="A15" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="27">
         <v>285.89999999999998</v>
       </c>
       <c r="C15" s="17">
@@ -2708,18 +3179,18 @@
         <f>C15*D15*0.08</f>
         <v>8148</v>
       </c>
-      <c r="F15" s="35">
-        <f>B15*D15</f>
+      <c r="F15" s="34">
+        <f t="shared" si="0"/>
         <v>1429.5</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <f>C15*D15*0.000048</f>
         <v>4.8887999999999998</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="27">
         <f>C15*D15*0.000024</f>
         <v>2.4443999999999999</v>
       </c>
@@ -2727,34 +3198,34 @@
         <v>5</v>
       </c>
       <c r="K15" s="17">
-        <f>(D15*J15)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="L15" s="20">
-        <f>F15/(H15+I15)</f>
+      <c r="L15" s="17">
+        <f t="shared" si="2"/>
         <v>194.93536246113567</v>
       </c>
-      <c r="M15" s="26">
-        <f>B15/C15</f>
+      <c r="M15" s="25">
+        <f t="shared" si="3"/>
         <v>1.4035346097201766E-2</v>
       </c>
       <c r="N15" s="17">
-        <f>F15/K15</f>
+        <f t="shared" si="4"/>
         <v>57.18</v>
       </c>
-      <c r="O15" s="26">
-        <f>F15/E15</f>
+      <c r="O15" s="25">
+        <f t="shared" si="5"/>
         <v>0.17544182621502208</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="25" customFormat="1">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:16" s="24" customFormat="1">
+      <c r="A16" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="27">
         <v>193.3</v>
       </c>
       <c r="C16" s="17">
@@ -2767,51 +3238,51 @@
         <f>C16*D16*0.07</f>
         <v>4929.7500000000009</v>
       </c>
-      <c r="F16" s="17">
-        <f>B16*D16</f>
+      <c r="F16" s="34">
+        <f t="shared" si="0"/>
         <v>966.5</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <v>3.6</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="27">
         <v>1.8</v>
       </c>
       <c r="J16" s="17">
         <v>5</v>
       </c>
       <c r="K16" s="17">
-        <f>(D16*J16)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="L16" s="20">
-        <f>F16/(H16+I16)</f>
+      <c r="L16" s="17">
+        <f t="shared" si="2"/>
         <v>178.98148148148147</v>
       </c>
-      <c r="M16" s="26">
-        <f>B16/C16</f>
+      <c r="M16" s="25">
+        <f t="shared" si="3"/>
         <v>1.3723819666311679E-2</v>
       </c>
       <c r="N16" s="17">
-        <f>F16/K16</f>
+        <f t="shared" si="4"/>
         <v>38.659999999999997</v>
       </c>
-      <c r="O16" s="26">
-        <f>F16/E16</f>
+      <c r="O16" s="25">
+        <f t="shared" si="5"/>
         <v>0.19605456666159538</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="25" customFormat="1">
+    <row r="17" spans="1:16" s="24" customFormat="1">
       <c r="A17" s="20" t="s">
         <v>374</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>45.1</v>
       </c>
       <c r="C17" s="17">
@@ -2825,39 +3296,39 @@
         <v>1450.8</v>
       </c>
       <c r="F17" s="17">
-        <f>B17*D17</f>
+        <f t="shared" si="0"/>
         <v>451</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="27">
         <v>1.8</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="27">
         <v>0.9</v>
       </c>
       <c r="J17" s="17">
         <v>1</v>
       </c>
       <c r="K17" s="17">
-        <f>(D17*J17)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L17" s="20">
-        <f>F17/(H17+I17)</f>
+      <c r="L17" s="17">
+        <f t="shared" si="2"/>
         <v>167.03703703703704</v>
       </c>
       <c r="M17" s="23">
-        <f>B17/C17</f>
+        <f t="shared" si="3"/>
         <v>1.8651778329197684E-2</v>
       </c>
       <c r="N17" s="17">
-        <f>F17/K17</f>
+        <f t="shared" si="4"/>
         <v>45.1</v>
       </c>
-      <c r="O17" s="24">
-        <f>F17/E17</f>
+      <c r="O17" s="25">
+        <f t="shared" si="5"/>
         <v>0.31086297215329473</v>
       </c>
       <c r="P17" s="5" t="s">
@@ -2868,7 +3339,7 @@
       <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="27">
         <v>54.1</v>
       </c>
       <c r="C18" s="17">
@@ -2882,48 +3353,48 @@
         <v>2135.7000000000003</v>
       </c>
       <c r="F18" s="17">
-        <f>B18*D18</f>
+        <f t="shared" si="0"/>
         <v>541</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="27">
         <v>1.8</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <v>1.8</v>
       </c>
       <c r="J18" s="17">
         <v>1</v>
       </c>
       <c r="K18" s="17">
-        <f>(D18*J18)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L18" s="20">
-        <f>F18/(H18+I18)</f>
+      <c r="L18" s="17">
+        <f t="shared" si="2"/>
         <v>150.27777777777777</v>
       </c>
       <c r="M18" s="23">
-        <f>B18/C18</f>
+        <f t="shared" si="3"/>
         <v>1.7731891183218617E-2</v>
       </c>
       <c r="N18" s="17">
-        <f>F18/K18</f>
+        <f t="shared" si="4"/>
         <v>54.1</v>
       </c>
-      <c r="O18" s="24">
-        <f>F18/E18</f>
+      <c r="O18" s="25">
+        <f t="shared" si="5"/>
         <v>0.25331273118883735</v>
       </c>
-      <c r="P18" s="25"/>
-    </row>
-    <row r="19" spans="1:16" s="25" customFormat="1">
-      <c r="A19" s="33" t="s">
+      <c r="P18" s="24"/>
+    </row>
+    <row r="19" spans="1:16" s="24" customFormat="1">
+      <c r="A19" s="32" t="s">
         <v>365</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="27">
         <v>106</v>
       </c>
       <c r="C19" s="17">
@@ -2937,50 +3408,50 @@
         <v>2411.5000000000005</v>
       </c>
       <c r="F19" s="17">
-        <f>B19*D19</f>
+        <f t="shared" si="0"/>
         <v>530</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="27">
         <v>2.4</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="27">
         <v>1.2</v>
       </c>
       <c r="J19" s="17">
         <v>5</v>
       </c>
       <c r="K19" s="17">
-        <f>(D19*J19)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="L19" s="20">
-        <f>F19/(H19+I19)</f>
+      <c r="L19" s="17">
+        <f t="shared" si="2"/>
         <v>147.22222222222223</v>
       </c>
-      <c r="M19" s="26">
-        <f>B19/C19</f>
+      <c r="M19" s="25">
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
-      <c r="N19" s="17">
-        <f>F19/K19</f>
+      <c r="N19" s="34">
+        <f t="shared" si="4"/>
         <v>21.2</v>
       </c>
-      <c r="O19" s="24">
-        <f>F19/E19</f>
+      <c r="O19" s="25">
+        <f t="shared" si="5"/>
         <v>0.21978021978021975</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="25" customFormat="1">
+    <row r="20" spans="1:16" s="24" customFormat="1">
       <c r="A20" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="27">
         <v>626.20000000000005</v>
       </c>
       <c r="C20" s="17">
@@ -2989,57 +3460,57 @@
       <c r="D20" s="17">
         <v>5</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="34">
         <f>C20*D20*0.07</f>
         <v>17976</v>
       </c>
-      <c r="F20" s="35">
-        <f>B20*D20</f>
+      <c r="F20" s="34">
+        <f t="shared" si="0"/>
         <v>3131</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="27">
         <f>C20*D20*0.00006</f>
         <v>15.408000000000001</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="27">
         <f>C20*D20*0.00003</f>
         <v>7.7040000000000006</v>
       </c>
       <c r="J20" s="17">
         <v>10</v>
       </c>
-      <c r="K20" s="17">
-        <f>(D20*J20)</f>
+      <c r="K20" s="34">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="L20" s="20">
-        <f>F20/(H20+I20)</f>
+      <c r="L20" s="17">
+        <f t="shared" si="2"/>
         <v>135.47075112495673</v>
       </c>
       <c r="M20" s="16">
-        <f>B20/C20</f>
+        <f t="shared" si="3"/>
         <v>1.2192367601246108E-2</v>
       </c>
       <c r="N20" s="17">
-        <f>F20/K20</f>
+        <f t="shared" si="4"/>
         <v>62.62</v>
       </c>
-      <c r="O20" s="26">
-        <f>F20/E20</f>
+      <c r="O20" s="25">
+        <f t="shared" si="5"/>
         <v>0.17417668001780151</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="27" customFormat="1">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:16" s="26" customFormat="1">
+      <c r="A21" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="27">
         <v>69.28</v>
       </c>
       <c r="C21" s="17">
@@ -3053,47 +3524,47 @@
         <v>3907.4000000000005</v>
       </c>
       <c r="F21" s="17">
-        <f>B21*D21</f>
+        <f t="shared" si="0"/>
         <v>692.8</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="27">
         <v>3</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="27">
         <v>3</v>
       </c>
       <c r="J21" s="17">
         <v>2</v>
       </c>
       <c r="K21" s="17">
-        <f>(D21*J21)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="L21" s="20">
-        <f>F21/(H21+I21)</f>
+      <c r="L21" s="17">
+        <f t="shared" si="2"/>
         <v>115.46666666666665</v>
       </c>
-      <c r="M21" s="26">
-        <f>B21/C21</f>
+      <c r="M21" s="25">
+        <f t="shared" si="3"/>
         <v>1.2411322106771767E-2</v>
       </c>
       <c r="N21" s="17">
-        <f>F21/K21</f>
+        <f t="shared" si="4"/>
         <v>34.64</v>
       </c>
-      <c r="O21" s="26">
-        <f>F21/E21</f>
+      <c r="O21" s="25">
+        <f t="shared" si="5"/>
         <v>0.17730460152531091</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="27" customFormat="1">
+    <row r="22" spans="1:16" s="26" customFormat="1">
       <c r="A22" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="27">
         <v>52.16</v>
       </c>
       <c r="C22" s="17">
@@ -3107,39 +3578,39 @@
         <v>2541.0000000000005</v>
       </c>
       <c r="F22" s="17">
-        <f>B22*D22</f>
+        <f t="shared" si="0"/>
         <v>521.59999999999991</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="27">
         <v>2.4</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="27">
         <v>2.4</v>
       </c>
       <c r="J22" s="17">
         <v>1</v>
       </c>
       <c r="K22" s="17">
-        <f>(D22*J22)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L22" s="20">
-        <f>F22/(H22+I22)</f>
+      <c r="L22" s="17">
+        <f t="shared" si="2"/>
         <v>108.66666666666666</v>
       </c>
-      <c r="M22" s="26">
-        <f>B22/C22</f>
+      <c r="M22" s="25">
+        <f t="shared" si="3"/>
         <v>1.4369146005509641E-2</v>
       </c>
       <c r="N22" s="17">
-        <f>F22/K22</f>
+        <f t="shared" si="4"/>
         <v>52.159999999999989</v>
       </c>
-      <c r="O22" s="26">
-        <f>F22/E22</f>
+      <c r="O22" s="25">
+        <f t="shared" si="5"/>
         <v>0.20527351436442337</v>
       </c>
     </row>
@@ -3147,7 +3618,7 @@
       <c r="A23" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="27">
         <v>55.04</v>
       </c>
       <c r="C23" s="17">
@@ -3161,39 +3632,39 @@
         <v>2578.5</v>
       </c>
       <c r="F23" s="17">
-        <f>B23*D23</f>
+        <f t="shared" si="0"/>
         <v>550.4</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="27">
         <v>3.6</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="27">
         <v>1.8</v>
       </c>
       <c r="J23" s="17">
         <v>1</v>
       </c>
       <c r="K23" s="17">
-        <f>(D23*J23)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L23" s="20">
-        <f>F23/(H23+I23)</f>
+      <c r="L23" s="17">
+        <f t="shared" si="2"/>
         <v>101.92592592592591</v>
       </c>
-      <c r="M23" s="26">
-        <f>B23/C23</f>
+      <c r="M23" s="25">
+        <f t="shared" si="3"/>
         <v>1.0672871824704284E-2</v>
       </c>
       <c r="N23" s="17">
-        <f>F23/K23</f>
+        <f t="shared" si="4"/>
         <v>55.04</v>
       </c>
-      <c r="O23" s="26">
-        <f>F23/E23</f>
+      <c r="O23" s="25">
+        <f t="shared" si="5"/>
         <v>0.21345743649408569</v>
       </c>
       <c r="P23" s="5" t="s">
@@ -3204,7 +3675,7 @@
       <c r="A24" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="27">
         <v>118.44</v>
       </c>
       <c r="C24" s="17">
@@ -3218,17 +3689,17 @@
         <v>3154.2000000000003</v>
       </c>
       <c r="F24" s="17">
-        <f>B24*D24</f>
+        <f t="shared" si="0"/>
         <v>592.20000000000005</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="27">
         <f>C24*D24*0.000072</f>
         <v>3.2443200000000001</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="27">
         <f>C24*D24*0.000072</f>
         <v>3.2443200000000001</v>
       </c>
@@ -3236,32 +3707,32 @@
         <v>1</v>
       </c>
       <c r="K24" s="17">
-        <f>(D24*J24)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L24" s="17">
-        <f>F24/(H24+I24)</f>
+        <f t="shared" si="2"/>
         <v>91.267199289835773</v>
       </c>
-      <c r="M24" s="26">
-        <f>B24/C24</f>
+      <c r="M24" s="25">
+        <f t="shared" si="3"/>
         <v>1.3142476697736351E-2</v>
       </c>
       <c r="N24" s="17">
-        <f>F24/K24</f>
+        <f t="shared" si="4"/>
         <v>118.44000000000001</v>
       </c>
-      <c r="O24" s="26">
-        <f>F24/E24</f>
+      <c r="O24" s="25">
+        <f t="shared" si="5"/>
         <v>0.1877496671105193</v>
       </c>
-      <c r="P24" s="27"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B25" s="27">
         <v>266.94</v>
       </c>
       <c r="C25" s="17">
@@ -3270,55 +3741,55 @@
       <c r="D25" s="17">
         <v>10</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="34">
         <f>C25*D25*0.11</f>
         <v>10652.4</v>
       </c>
-      <c r="F25" s="35">
-        <f>B25*D25</f>
+      <c r="F25" s="34">
+        <f t="shared" si="0"/>
         <v>2669.4</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H25" s="28">
+      <c r="H25" s="27">
         <v>12</v>
       </c>
-      <c r="I25" s="28">
+      <c r="I25" s="27">
         <v>18</v>
       </c>
       <c r="J25" s="17">
         <v>1</v>
       </c>
       <c r="K25" s="17">
-        <f>(D25*J25)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L25" s="17">
-        <f>F25/(H25+I25)</f>
+        <f t="shared" si="2"/>
         <v>88.98</v>
       </c>
-      <c r="M25" s="26">
-        <f>B25/C25</f>
+      <c r="M25" s="25">
+        <f t="shared" si="3"/>
         <v>2.7565055762081785E-2</v>
       </c>
       <c r="N25" s="17">
-        <f>F25/K25</f>
+        <f t="shared" si="4"/>
         <v>266.94</v>
       </c>
-      <c r="O25" s="24">
-        <f>F25/E25</f>
+      <c r="O25" s="25">
+        <f t="shared" si="5"/>
         <v>0.25059141601892532</v>
       </c>
-      <c r="P25" s="30" t="s">
-        <v>412</v>
+      <c r="P25" s="29" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="27">
         <v>62</v>
       </c>
       <c r="C26" s="17">
@@ -3332,17 +3803,17 @@
         <v>2449.6</v>
       </c>
       <c r="F26" s="17">
-        <f>B26*D26</f>
+        <f t="shared" si="0"/>
         <v>620</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>413</v>
-      </c>
-      <c r="H26" s="28">
+        <v>412</v>
+      </c>
+      <c r="H26" s="27">
         <f>C26*D26*0.00012</f>
         <v>3.6743999999999999</v>
       </c>
-      <c r="I26" s="28">
+      <c r="I26" s="27">
         <f>C26*D26*0.00012</f>
         <v>3.6743999999999999</v>
       </c>
@@ -3350,32 +3821,32 @@
         <v>2</v>
       </c>
       <c r="K26" s="17">
-        <f>(D26*J26)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="L26" s="17">
-        <f>F26/(H26+I26)</f>
+        <f t="shared" si="2"/>
         <v>84.36751578489006</v>
       </c>
       <c r="M26" s="23">
-        <f>B26/C26</f>
+        <f t="shared" si="3"/>
         <v>2.0248203788373612E-2</v>
       </c>
       <c r="N26" s="17">
-        <f>F26/K26</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="O26" s="24">
-        <f>F26/E26</f>
+      <c r="O26" s="25">
+        <f t="shared" si="5"/>
         <v>0.25310254735467014</v>
       </c>
-      <c r="P26" s="27"/>
+      <c r="P26" s="26"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="27">
         <v>72.040000000000006</v>
       </c>
       <c r="C27" s="17">
@@ -3389,17 +3860,17 @@
         <v>3329.1</v>
       </c>
       <c r="F27" s="17">
-        <f>B27*D27</f>
+        <f t="shared" si="0"/>
         <v>720.40000000000009</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>413</v>
-      </c>
-      <c r="H27" s="28">
+        <v>412</v>
+      </c>
+      <c r="H27" s="27">
         <f>C27*D27*0.00012</f>
         <v>4.4388000000000005</v>
       </c>
-      <c r="I27" s="28">
+      <c r="I27" s="27">
         <f>C27*D27*0.00012</f>
         <v>4.4388000000000005</v>
       </c>
@@ -3407,32 +3878,32 @@
         <v>1</v>
       </c>
       <c r="K27" s="17">
-        <f>(D27*J27)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L27" s="17">
-        <f>F27/(H27+I27)</f>
+        <f t="shared" si="2"/>
         <v>81.14805803370281</v>
       </c>
       <c r="M27" s="23">
-        <f>B27/C27</f>
+        <f t="shared" si="3"/>
         <v>1.9475533928088675E-2</v>
       </c>
       <c r="N27" s="17">
-        <f>F27/K27</f>
+        <f t="shared" si="4"/>
         <v>72.040000000000006</v>
       </c>
-      <c r="O27" s="24">
-        <f>F27/E27</f>
+      <c r="O27" s="25">
+        <f t="shared" si="5"/>
         <v>0.21639482142320751</v>
       </c>
-      <c r="P27" s="27"/>
+      <c r="P27" s="26"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="27">
         <v>70.44</v>
       </c>
       <c r="C28" s="17">
@@ -3446,17 +3917,17 @@
         <v>3062.4</v>
       </c>
       <c r="F28" s="17">
-        <f>B28*D28</f>
+        <f t="shared" si="0"/>
         <v>704.4</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>413</v>
-      </c>
-      <c r="H28" s="28">
+        <v>412</v>
+      </c>
+      <c r="H28" s="27">
         <f>C28*D28*0.00012</f>
         <v>4.5936000000000003</v>
       </c>
-      <c r="I28" s="28">
+      <c r="I28" s="27">
         <f>C28*D28*0.00012</f>
         <v>4.5936000000000003</v>
       </c>
@@ -3464,23 +3935,23 @@
         <v>1</v>
       </c>
       <c r="K28" s="17">
-        <f>(D28*J28)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L28" s="17">
-        <f>F28/(H28+I28)</f>
+      <c r="L28" s="34">
+        <f t="shared" si="2"/>
         <v>76.671891327063733</v>
       </c>
       <c r="M28" s="23">
-        <f>B28/C28</f>
+        <f t="shared" si="3"/>
         <v>1.8401253918495297E-2</v>
       </c>
       <c r="N28" s="17">
-        <f>F28/K28</f>
+        <f t="shared" si="4"/>
         <v>70.44</v>
       </c>
-      <c r="O28" s="24">
-        <f>F28/E28</f>
+      <c r="O28" s="25">
+        <f t="shared" si="5"/>
         <v>0.23001567398119122</v>
       </c>
       <c r="P28" s="4"/>
@@ -3489,7 +3960,7 @@
       <c r="A29" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="27">
         <v>34.159999999999997</v>
       </c>
       <c r="C29" s="17">
@@ -3503,17 +3974,17 @@
         <v>3376.7999999999997</v>
       </c>
       <c r="F29" s="17">
-        <f>B29*D29</f>
+        <f t="shared" si="0"/>
         <v>512.4</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="H29" s="28">
+      <c r="H29" s="27">
         <f>C29*D29*0.00006</f>
         <v>3.3768000000000002</v>
       </c>
-      <c r="I29" s="28">
+      <c r="I29" s="27">
         <f>C29*D29*0.00006</f>
         <v>3.3768000000000002</v>
       </c>
@@ -3521,32 +3992,32 @@
         <v>1</v>
       </c>
       <c r="K29" s="17">
-        <f>(D29*J29)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="L29" s="17">
-        <f>F29/(H29+I29)</f>
+      <c r="L29" s="34">
+        <f t="shared" si="2"/>
         <v>75.870646766169145</v>
       </c>
       <c r="M29" s="16">
-        <f>B29/C29</f>
+        <f t="shared" si="3"/>
         <v>9.1044776119402968E-3</v>
       </c>
       <c r="N29" s="17">
-        <f>F29/K29</f>
+        <f t="shared" si="4"/>
         <v>34.159999999999997</v>
       </c>
-      <c r="O29" s="34">
-        <f>F29/E29</f>
+      <c r="O29" s="33">
+        <f t="shared" si="5"/>
         <v>0.15174129353233831</v>
       </c>
-      <c r="P29" s="27"/>
+      <c r="P29" s="26"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="17" t="s">
-        <v>414</v>
-      </c>
-      <c r="B30" s="28">
+      <c r="A30" s="36" t="s">
+        <v>413</v>
+      </c>
+      <c r="B30" s="27">
         <v>45.02</v>
       </c>
       <c r="C30" s="17">
@@ -3560,50 +4031,50 @@
         <v>1891.4</v>
       </c>
       <c r="F30" s="17">
-        <f>B30*D30</f>
+        <f t="shared" si="0"/>
         <v>450.20000000000005</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="27">
         <v>2.4</v>
       </c>
-      <c r="I30" s="28">
+      <c r="I30" s="27">
         <v>4.8</v>
       </c>
       <c r="J30" s="17">
         <v>1</v>
       </c>
       <c r="K30" s="17">
-        <f>(D30*J30)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L30" s="17">
-        <f>F30/(H30+I30)</f>
+      <c r="L30" s="34">
+        <f t="shared" si="2"/>
         <v>62.527777777777793</v>
       </c>
       <c r="M30" s="23">
-        <f>B30/C30</f>
+        <f t="shared" si="3"/>
         <v>1.6661732050333087E-2</v>
       </c>
       <c r="N30" s="17">
-        <f>F30/K30</f>
+        <f t="shared" si="4"/>
         <v>45.02</v>
       </c>
-      <c r="O30" s="24">
-        <f>F30/E30</f>
+      <c r="O30" s="25">
+        <f t="shared" si="5"/>
         <v>0.23802474357618697</v>
       </c>
-      <c r="P30" s="36" t="s">
-        <v>417</v>
+      <c r="P30" s="35" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="27">
         <v>61.2</v>
       </c>
       <c r="C31" s="17">
@@ -3617,39 +4088,39 @@
         <v>1685.3999999999999</v>
       </c>
       <c r="F31" s="17">
-        <f>B31*D31</f>
+        <f t="shared" si="0"/>
         <v>306</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H31" s="28">
+      <c r="H31" s="27">
         <v>3.6</v>
       </c>
-      <c r="I31" s="28">
+      <c r="I31" s="27">
         <v>1.8</v>
       </c>
       <c r="J31" s="17">
         <v>2</v>
       </c>
       <c r="K31" s="17">
-        <f>(D31*J31)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L31" s="17">
-        <f>F31/(H31+I31)</f>
+      <c r="L31" s="34">
+        <f t="shared" si="2"/>
         <v>56.666666666666664</v>
       </c>
-      <c r="M31" s="26">
-        <f>B31/C31</f>
+      <c r="M31" s="25">
+        <f t="shared" si="3"/>
         <v>1.0893556425774298E-2</v>
       </c>
       <c r="N31" s="17">
-        <f>F31/K31</f>
+        <f t="shared" si="4"/>
         <v>30.6</v>
       </c>
-      <c r="O31" s="26">
-        <f>F31/E31</f>
+      <c r="O31" s="25">
+        <f t="shared" si="5"/>
         <v>0.18155927376290495</v>
       </c>
       <c r="P31" s="5" t="s">
@@ -3657,10 +4128,10 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="36" t="s">
         <v>381</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="27">
         <v>11.56</v>
       </c>
       <c r="C32" s="17">
@@ -3674,39 +4145,39 @@
         <v>1243.2</v>
       </c>
       <c r="F32" s="17">
-        <f>B32*D32</f>
+        <f t="shared" si="0"/>
         <v>115.60000000000001</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H32" s="28">
+      <c r="H32" s="27">
         <v>1.44</v>
       </c>
-      <c r="I32" s="28">
+      <c r="I32" s="27">
         <v>0.72</v>
       </c>
       <c r="J32" s="17">
         <v>1</v>
       </c>
       <c r="K32" s="17">
-        <f>(D32*J32)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L32" s="17">
-        <f>F32/(H32+I32)</f>
+      <c r="L32" s="34">
+        <f t="shared" si="2"/>
         <v>53.518518518518519</v>
       </c>
       <c r="M32" s="16">
-        <f>B32/C32</f>
+        <f t="shared" si="3"/>
         <v>6.5090090090090093E-3</v>
       </c>
-      <c r="N32" s="35">
-        <f>F32/K32</f>
+      <c r="N32" s="34">
+        <f t="shared" si="4"/>
         <v>11.56</v>
       </c>
-      <c r="O32" s="34">
-        <f>F32/E32</f>
+      <c r="O32" s="33">
+        <f t="shared" si="5"/>
         <v>9.298584298584299E-2</v>
       </c>
       <c r="P32" s="5" t="s">
@@ -3714,10 +4185,10 @@
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="36" t="s">
         <v>382</v>
       </c>
-      <c r="B33" s="28">
+      <c r="B33" s="27">
         <v>68.12</v>
       </c>
       <c r="C33" s="17">
@@ -3731,17 +4202,17 @@
         <v>3376</v>
       </c>
       <c r="F33" s="17">
-        <f>B33*D33</f>
+        <f t="shared" si="0"/>
         <v>681.2</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="H33" s="28">
+      <c r="H33" s="27">
         <f>C33*D33*0.00018</f>
         <v>7.5960000000000001</v>
       </c>
-      <c r="I33" s="28">
+      <c r="I33" s="27">
         <f>C33*D33*0.00018</f>
         <v>7.5960000000000001</v>
       </c>
@@ -3749,32 +4220,32 @@
         <v>1</v>
       </c>
       <c r="K33" s="17">
-        <f>(D33*J33)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L33" s="17">
-        <f>F33/(H33+I33)</f>
+      <c r="L33" s="34">
+        <f t="shared" si="2"/>
         <v>44.839389152185362</v>
       </c>
       <c r="M33" s="23">
-        <f>B33/C33</f>
+        <f t="shared" si="3"/>
         <v>1.614218009478673E-2</v>
       </c>
       <c r="N33" s="17">
-        <f>F33/K33</f>
+        <f t="shared" si="4"/>
         <v>68.12</v>
       </c>
-      <c r="O33" s="26">
-        <f>F33/E33</f>
+      <c r="O33" s="25">
+        <f t="shared" si="5"/>
         <v>0.20177725118483414</v>
       </c>
-      <c r="P33" s="27"/>
+      <c r="P33" s="26"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="36" t="s">
         <v>384</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="27">
         <v>21.26</v>
       </c>
       <c r="C34" s="17">
@@ -3788,43 +4259,43 @@
         <v>2013.2000000000003</v>
       </c>
       <c r="F34" s="17">
-        <f>B34*D34</f>
+        <f t="shared" si="0"/>
         <v>425.20000000000005</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="H34" s="28">
+      <c r="H34" s="27">
         <v>3.6</v>
       </c>
-      <c r="I34" s="28">
+      <c r="I34" s="27">
         <v>13.8</v>
       </c>
       <c r="J34" s="17">
         <v>1</v>
       </c>
       <c r="K34" s="17">
-        <f>(D34*J34)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="L34" s="17">
-        <f>F34/(H34+I34)</f>
+      <c r="L34" s="34">
+        <f t="shared" si="2"/>
         <v>24.436781609195403</v>
       </c>
-      <c r="M34" s="26">
-        <f>B34/C34</f>
+      <c r="M34" s="25">
+        <f t="shared" si="3"/>
         <v>1.4784422809457581E-2</v>
       </c>
-      <c r="N34" s="17">
-        <f>F34/K34</f>
+      <c r="N34" s="34">
+        <f t="shared" si="4"/>
         <v>21.26</v>
       </c>
-      <c r="O34" s="26">
-        <f>F34/E34</f>
+      <c r="O34" s="25">
+        <f t="shared" si="5"/>
         <v>0.21120604013510827</v>
       </c>
-      <c r="P34" s="30" t="s">
-        <v>412</v>
+      <c r="P34" s="29" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -3835,15 +4306,15 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
       <c r="O35" s="3"/>
-      <c r="P35" s="27"/>
+      <c r="P35" s="26"/>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="19" t="s">
@@ -3858,8 +4329,8 @@
         <v>623.40000000000009</v>
       </c>
       <c r="G36" s="17"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
       <c r="L36" s="17">
@@ -3874,11 +4345,11 @@
         <f>MEDIAN(N10:N34)</f>
         <v>55.04</v>
       </c>
-      <c r="O36" s="26">
+      <c r="O36" s="25">
         <f>MEDIAN(O10:O34)</f>
         <v>0.21345743649408569</v>
       </c>
-      <c r="P36" s="27"/>
+      <c r="P36" s="26"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="17"/>
@@ -3888,8 +4359,8 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
@@ -3903,8 +4374,8 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
@@ -3918,8 +4389,8 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
@@ -3933,8 +4404,8 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -4116,10 +4587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD115"/>
+  <dimension ref="A1:AD134"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127:B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4176,6 +4647,7 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29">
+      <c r="A5" s="40"/>
       <c r="B5" t="s">
         <v>89</v>
       </c>
@@ -5642,7 +6114,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="113" spans="2:15">
+    <row r="113" spans="1:15">
       <c r="B113" t="s">
         <v>154</v>
       </c>
@@ -5654,7 +6126,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="114" spans="2:15">
+    <row r="114" spans="1:15">
       <c r="B114" t="s">
         <v>155</v>
       </c>
@@ -5666,7 +6138,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="115" spans="2:15">
+    <row r="115" spans="1:15">
       <c r="B115" t="s">
         <v>156</v>
       </c>
@@ -5675,6 +6147,114 @@
       </c>
       <c r="O115" t="s">
         <v>332</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
+      <c r="A117" s="37" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
+      <c r="A118" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B118" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="A119" s="37"/>
+      <c r="B119" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="A120" s="37"/>
+      <c r="B120" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" s="37"/>
+      <c r="B121" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
+      <c r="A122" s="37"/>
+      <c r="B122" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15">
+      <c r="A123" s="37"/>
+      <c r="B123" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15">
+      <c r="A124" s="37"/>
+      <c r="B124" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15">
+      <c r="A125" s="37"/>
+      <c r="B125" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="A126" s="37"/>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="A127" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15">
+      <c r="A128" s="37"/>
+      <c r="B128" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="37"/>
+      <c r="B129" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="37"/>
+      <c r="B130" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="37"/>
+      <c r="B131" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="37"/>
+      <c r="B132" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="37"/>
+      <c r="B133" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="37"/>
+      <c r="B134" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -5682,4 +6262,2314 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O115"/>
+  <sheetViews>
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80:O87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="B1" s="40" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="B2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="G2" s="11" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="N3" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="B4" t="s">
+        <v>424</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="N4" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="40" t="s">
+        <v>503</v>
+      </c>
+      <c r="B5" t="s">
+        <v>425</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>504</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="N5" s="40" t="s">
+        <v>504</v>
+      </c>
+      <c r="O5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="37"/>
+      <c r="B6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="N6" s="40" t="s">
+        <v>505</v>
+      </c>
+      <c r="O6" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="37"/>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="37"/>
+      <c r="B8" t="s">
+        <v>427</v>
+      </c>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="37"/>
+      <c r="B9" t="s">
+        <v>428</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="37"/>
+      <c r="B10" t="s">
+        <v>429</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="37"/>
+      <c r="B11" t="s">
+        <v>430</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="N12" s="37"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>493</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="N13" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="37"/>
+      <c r="B14" t="s">
+        <v>494</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="37"/>
+      <c r="B15" t="s">
+        <v>495</v>
+      </c>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="37"/>
+      <c r="B16" t="s">
+        <v>496</v>
+      </c>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="37"/>
+      <c r="B17" t="s">
+        <v>497</v>
+      </c>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="N17" s="37"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="37"/>
+      <c r="B18" t="s">
+        <v>498</v>
+      </c>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="37"/>
+      <c r="B19" t="s">
+        <v>499</v>
+      </c>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="37"/>
+      <c r="B20" t="s">
+        <v>500</v>
+      </c>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="N21" s="40"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="N22" s="37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="B23" t="s">
+        <v>431</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="N23" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="37"/>
+      <c r="B24" t="s">
+        <v>432</v>
+      </c>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="37"/>
+      <c r="B25" t="s">
+        <v>433</v>
+      </c>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="37"/>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="37"/>
+      <c r="B27" t="s">
+        <v>434</v>
+      </c>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="37"/>
+      <c r="B28" t="s">
+        <v>435</v>
+      </c>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="37"/>
+      <c r="B29" t="s">
+        <v>436</v>
+      </c>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="37"/>
+      <c r="B30" t="s">
+        <v>437</v>
+      </c>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="N30" s="37"/>
+      <c r="O30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="N31" s="37"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="N32" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="N33" s="37"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="N34" s="37"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="N35" s="37"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="N36" s="37"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="N37" s="37"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="N38" s="37"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="N39" s="37"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="N40" s="37"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="N41" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="B42" t="s">
+        <v>439</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="N42" s="40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="37"/>
+      <c r="B43" t="s">
+        <v>440</v>
+      </c>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+      <c r="N43" s="37"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="37"/>
+      <c r="B44" t="s">
+        <v>441</v>
+      </c>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="N44" s="37"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="37"/>
+      <c r="B45" t="s">
+        <v>442</v>
+      </c>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="N45" s="37"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="37"/>
+      <c r="B46" t="s">
+        <v>443</v>
+      </c>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="N46" s="37"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="37"/>
+      <c r="B47" t="s">
+        <v>444</v>
+      </c>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="N47" s="37"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="37"/>
+      <c r="B48" t="s">
+        <v>445</v>
+      </c>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="N48" s="37"/>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="37"/>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="N49" s="37"/>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="N50" s="37"/>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>486</v>
+      </c>
+      <c r="G51" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="N51" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="37"/>
+      <c r="B52" t="s">
+        <v>487</v>
+      </c>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="N52" s="37"/>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="37"/>
+      <c r="B53" t="s">
+        <v>488</v>
+      </c>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="N53" s="37"/>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="37"/>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="N54" s="37"/>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="37"/>
+      <c r="B55" t="s">
+        <v>489</v>
+      </c>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="N55" s="37"/>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="37"/>
+      <c r="B56" t="s">
+        <v>490</v>
+      </c>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="N56" s="37"/>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="37"/>
+      <c r="B57" t="s">
+        <v>491</v>
+      </c>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="N57" s="37"/>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="37"/>
+      <c r="B58" t="s">
+        <v>492</v>
+      </c>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="N58" s="37"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="N59" s="37"/>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
+      <c r="N60" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>446</v>
+      </c>
+      <c r="G61" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+      <c r="N61" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="O61" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" s="37"/>
+      <c r="B62" t="s">
+        <v>447</v>
+      </c>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="N62" s="37"/>
+      <c r="O62" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" s="37"/>
+      <c r="B63" t="s">
+        <v>448</v>
+      </c>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" s="37"/>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="A65" s="37"/>
+      <c r="B65" t="s">
+        <v>449</v>
+      </c>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="A66" s="37"/>
+      <c r="B66" t="s">
+        <v>450</v>
+      </c>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+      <c r="L66" s="37"/>
+      <c r="N66" s="37"/>
+      <c r="O66" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
+      <c r="A67" s="37"/>
+      <c r="B67" t="s">
+        <v>451</v>
+      </c>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="A68" s="37"/>
+      <c r="B68" t="s">
+        <v>452</v>
+      </c>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
+      <c r="A69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37"/>
+      <c r="N69" s="37"/>
+    </row>
+    <row r="70" spans="1:15">
+      <c r="A70" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>480</v>
+      </c>
+      <c r="G70" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="37"/>
+      <c r="N70" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="A71" s="37"/>
+      <c r="B71" t="s">
+        <v>481</v>
+      </c>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
+      <c r="K71" s="37"/>
+      <c r="L71" s="37"/>
+      <c r="N71" s="37"/>
+    </row>
+    <row r="72" spans="1:15">
+      <c r="A72" s="37"/>
+      <c r="B72" t="s">
+        <v>482</v>
+      </c>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="37"/>
+      <c r="N72" s="37"/>
+    </row>
+    <row r="73" spans="1:15">
+      <c r="A73" s="37"/>
+      <c r="B73" t="s">
+        <v>125</v>
+      </c>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="37"/>
+      <c r="L73" s="37"/>
+      <c r="N73" s="37"/>
+    </row>
+    <row r="74" spans="1:15">
+      <c r="A74" s="37"/>
+      <c r="B74" t="s">
+        <v>483</v>
+      </c>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
+      <c r="L74" s="37"/>
+      <c r="N74" s="37"/>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="A75" s="37"/>
+      <c r="B75" t="s">
+        <v>484</v>
+      </c>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="37"/>
+      <c r="L75" s="37"/>
+      <c r="N75" s="37"/>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="A76" s="37"/>
+      <c r="B76" t="s">
+        <v>485</v>
+      </c>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="37"/>
+      <c r="L76" s="37"/>
+      <c r="N76" s="37"/>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="A77" s="37"/>
+      <c r="B77" t="s">
+        <v>129</v>
+      </c>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="I77" s="37"/>
+      <c r="J77" s="37"/>
+      <c r="K77" s="37"/>
+      <c r="L77" s="37"/>
+      <c r="N77" s="37"/>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="A78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="37"/>
+      <c r="K78" s="37"/>
+      <c r="L78" s="37"/>
+      <c r="N78" s="37"/>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="A79" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G79" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
+      <c r="L79" s="37"/>
+      <c r="N79" s="37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
+      <c r="A80" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" t="s">
+        <v>453</v>
+      </c>
+      <c r="G80" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I80" s="37"/>
+      <c r="J80" s="37"/>
+      <c r="K80" s="37"/>
+      <c r="L80" s="37"/>
+      <c r="N80" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="O80" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" s="37"/>
+      <c r="B81" t="s">
+        <v>454</v>
+      </c>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="I81" s="37"/>
+      <c r="J81" s="37"/>
+      <c r="K81" s="37"/>
+      <c r="L81" s="37"/>
+      <c r="N81" s="37"/>
+      <c r="O81" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="A82" s="37"/>
+      <c r="B82" t="s">
+        <v>455</v>
+      </c>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
+      <c r="K82" s="37"/>
+      <c r="L82" s="37"/>
+      <c r="N82" s="37"/>
+      <c r="O82" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" s="37"/>
+      <c r="B83" t="s">
+        <v>139</v>
+      </c>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37"/>
+      <c r="K83" s="37"/>
+      <c r="L83" s="37"/>
+      <c r="N83" s="37"/>
+      <c r="O83" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" s="37"/>
+      <c r="B84" t="s">
+        <v>456</v>
+      </c>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="I84" s="37"/>
+      <c r="J84" s="37"/>
+      <c r="K84" s="37"/>
+      <c r="L84" s="37"/>
+      <c r="N84" s="37"/>
+      <c r="O84" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
+      <c r="A85" s="37"/>
+      <c r="B85" t="s">
+        <v>457</v>
+      </c>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="I85" s="37"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="37"/>
+      <c r="L85" s="37"/>
+      <c r="N85" s="37"/>
+      <c r="O85" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
+      <c r="A86" s="37"/>
+      <c r="B86" t="s">
+        <v>458</v>
+      </c>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
+      <c r="N86" s="37"/>
+      <c r="O86" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="A87" s="37"/>
+      <c r="B87" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="I87" s="37"/>
+      <c r="J87" s="37"/>
+      <c r="K87" s="37"/>
+      <c r="L87" s="37"/>
+      <c r="N87" s="37"/>
+      <c r="O87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
+      <c r="A88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="37"/>
+      <c r="K88" s="37"/>
+      <c r="L88" s="37"/>
+      <c r="N88" s="37"/>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" t="s">
+        <v>473</v>
+      </c>
+      <c r="G89" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H89" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="I89" s="37"/>
+      <c r="J89" s="37"/>
+      <c r="K89" s="37"/>
+      <c r="L89" s="37"/>
+      <c r="N89" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
+      <c r="A90" s="37"/>
+      <c r="B90" t="s">
+        <v>474</v>
+      </c>
+      <c r="G90" s="37"/>
+      <c r="H90" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="I90" s="37"/>
+      <c r="J90" s="37"/>
+      <c r="K90" s="37"/>
+      <c r="L90" s="37"/>
+      <c r="N90" s="37"/>
+    </row>
+    <row r="91" spans="1:15">
+      <c r="A91" s="37"/>
+      <c r="B91" t="s">
+        <v>475</v>
+      </c>
+      <c r="G91" s="37"/>
+      <c r="H91" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="I91" s="37"/>
+      <c r="J91" s="37"/>
+      <c r="K91" s="37"/>
+      <c r="L91" s="37"/>
+      <c r="N91" s="37"/>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="A92" s="37"/>
+      <c r="B92" t="s">
+        <v>29</v>
+      </c>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I92" s="37"/>
+      <c r="J92" s="37"/>
+      <c r="K92" s="37"/>
+      <c r="L92" s="37"/>
+      <c r="N92" s="37"/>
+    </row>
+    <row r="93" spans="1:15">
+      <c r="A93" s="37"/>
+      <c r="B93" t="s">
+        <v>476</v>
+      </c>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="I93" s="37"/>
+      <c r="J93" s="37"/>
+      <c r="K93" s="37"/>
+      <c r="L93" s="37"/>
+      <c r="N93" s="37"/>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="A94" s="37"/>
+      <c r="B94" t="s">
+        <v>477</v>
+      </c>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="I94" s="37"/>
+      <c r="J94" s="37"/>
+      <c r="K94" s="37"/>
+      <c r="L94" s="37"/>
+      <c r="N94" s="37"/>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="A95" s="37"/>
+      <c r="B95" t="s">
+        <v>478</v>
+      </c>
+      <c r="G95" s="37"/>
+      <c r="H95" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="I95" s="37"/>
+      <c r="J95" s="37"/>
+      <c r="K95" s="37"/>
+      <c r="L95" s="37"/>
+      <c r="N95" s="37"/>
+    </row>
+    <row r="96" spans="1:15">
+      <c r="A96" s="37"/>
+      <c r="B96" t="s">
+        <v>479</v>
+      </c>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="I96" s="37"/>
+      <c r="J96" s="37"/>
+      <c r="K96" s="37"/>
+      <c r="L96" s="37"/>
+      <c r="N96" s="37"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="A97" s="37"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="37"/>
+      <c r="K97" s="37"/>
+      <c r="L97" s="37"/>
+      <c r="N97" s="37"/>
+    </row>
+    <row r="98" spans="1:14">
+      <c r="A98" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G98" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="37"/>
+      <c r="K98" s="37"/>
+      <c r="L98" s="37"/>
+      <c r="N98" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
+      <c r="A99" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>459</v>
+      </c>
+      <c r="G99" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H99" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
+      <c r="K99" s="37"/>
+      <c r="L99" s="37"/>
+      <c r="N99" s="40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="A100" s="37"/>
+      <c r="B100" t="s">
+        <v>460</v>
+      </c>
+      <c r="G100" s="37"/>
+      <c r="H100" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="I100" s="37"/>
+      <c r="J100" s="37"/>
+      <c r="K100" s="37"/>
+      <c r="L100" s="37"/>
+      <c r="N100" s="37"/>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="37"/>
+      <c r="B101" t="s">
+        <v>461</v>
+      </c>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="I101" s="37"/>
+      <c r="J101" s="37"/>
+      <c r="K101" s="37"/>
+      <c r="L101" s="37"/>
+      <c r="N101" s="37"/>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="37"/>
+      <c r="B102" t="s">
+        <v>462</v>
+      </c>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="I102" s="37"/>
+      <c r="J102" s="37"/>
+      <c r="K102" s="37"/>
+      <c r="L102" s="37"/>
+      <c r="N102" s="37"/>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="37"/>
+      <c r="B103" t="s">
+        <v>463</v>
+      </c>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="I103" s="37"/>
+      <c r="J103" s="37"/>
+      <c r="K103" s="37"/>
+      <c r="L103" s="37"/>
+      <c r="N103" s="37"/>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="A104" s="37"/>
+      <c r="B104" t="s">
+        <v>464</v>
+      </c>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="I104" s="37"/>
+      <c r="J104" s="37"/>
+      <c r="K104" s="37"/>
+      <c r="L104" s="37"/>
+      <c r="N104" s="37"/>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="A105" s="37"/>
+      <c r="B105" t="s">
+        <v>465</v>
+      </c>
+      <c r="G105" s="37"/>
+      <c r="H105" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="I105" s="37"/>
+      <c r="J105" s="37"/>
+      <c r="K105" s="37"/>
+      <c r="L105" s="37"/>
+      <c r="N105" s="37"/>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="A106" s="37"/>
+      <c r="B106" t="s">
+        <v>466</v>
+      </c>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I106" s="37"/>
+      <c r="J106" s="37"/>
+      <c r="K106" s="37"/>
+      <c r="L106" s="37"/>
+      <c r="N106" s="37"/>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="A107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="37"/>
+      <c r="K107" s="37"/>
+      <c r="L107" s="37"/>
+      <c r="N107" s="37"/>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="A108" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108" t="s">
+        <v>467</v>
+      </c>
+      <c r="G108" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H108" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I108" s="37"/>
+      <c r="J108" s="37"/>
+      <c r="K108" s="37"/>
+      <c r="L108" s="37"/>
+      <c r="N108" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" s="37"/>
+      <c r="B109" t="s">
+        <v>468</v>
+      </c>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="I109" s="37"/>
+      <c r="J109" s="37"/>
+      <c r="K109" s="37"/>
+      <c r="L109" s="37"/>
+      <c r="N109" s="37"/>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="A110" s="37"/>
+      <c r="B110" t="s">
+        <v>469</v>
+      </c>
+      <c r="G110" s="37"/>
+      <c r="H110" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="I110" s="37"/>
+      <c r="J110" s="37"/>
+      <c r="K110" s="37"/>
+      <c r="L110" s="37"/>
+      <c r="N110" s="37"/>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="A111" s="37"/>
+      <c r="B111" t="s">
+        <v>152</v>
+      </c>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="I111" s="37"/>
+      <c r="J111" s="37"/>
+      <c r="K111" s="37"/>
+      <c r="L111" s="37"/>
+      <c r="N111" s="37"/>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="A112" s="37"/>
+      <c r="B112" t="s">
+        <v>470</v>
+      </c>
+      <c r="G112" s="37"/>
+      <c r="H112" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="I112" s="37"/>
+      <c r="J112" s="37"/>
+      <c r="K112" s="37"/>
+      <c r="L112" s="37"/>
+      <c r="N112" s="37"/>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="A113" s="37"/>
+      <c r="B113" t="s">
+        <v>471</v>
+      </c>
+      <c r="G113" s="37"/>
+      <c r="H113" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="I113" s="37"/>
+      <c r="J113" s="37"/>
+      <c r="K113" s="37"/>
+      <c r="L113" s="37"/>
+      <c r="N113" s="37"/>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="37"/>
+      <c r="B114" t="s">
+        <v>472</v>
+      </c>
+      <c r="G114" s="37"/>
+      <c r="H114" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="I114" s="37"/>
+      <c r="J114" s="37"/>
+      <c r="K114" s="37"/>
+      <c r="L114" s="37"/>
+      <c r="N114" s="37"/>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="A115" s="37"/>
+      <c r="B115" t="s">
+        <v>156</v>
+      </c>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="I115" s="37"/>
+      <c r="J115" s="37"/>
+      <c r="K115" s="37"/>
+      <c r="L115" s="37"/>
+      <c r="N115" s="37"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="40" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>419</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>420</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>421</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>420</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="37">
+        <v>1</v>
+      </c>
+      <c r="B3" s="37">
+        <v>250358</v>
+      </c>
+      <c r="C3" s="39">
+        <v>0.50061187273047203</v>
+      </c>
+      <c r="D3" s="37">
+        <v>250358</v>
+      </c>
+      <c r="E3" s="39">
+        <v>0.50061187273047203</v>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="37">
+        <v>2</v>
+      </c>
+      <c r="B4" s="37">
+        <v>124661</v>
+      </c>
+      <c r="C4" s="39">
+        <v>0.24927015180842385</v>
+      </c>
+      <c r="D4" s="37">
+        <v>375019</v>
+      </c>
+      <c r="E4" s="39">
+        <v>0.74988202453889596</v>
+      </c>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="37">
+        <v>3</v>
+      </c>
+      <c r="B5" s="37">
+        <v>62537</v>
+      </c>
+      <c r="C5" s="39">
+        <v>0.12504799001807623</v>
+      </c>
+      <c r="D5" s="37">
+        <v>437556</v>
+      </c>
+      <c r="E5" s="39">
+        <v>0.87493001455697217</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="37">
+        <v>4</v>
+      </c>
+      <c r="B6" s="37">
+        <v>31180</v>
+      </c>
+      <c r="C6" s="39">
+        <v>6.2347031817381986E-2</v>
+      </c>
+      <c r="D6" s="37">
+        <v>468736</v>
+      </c>
+      <c r="E6" s="39">
+        <v>0.93727704637435416</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="40" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="37">
+        <v>5</v>
+      </c>
+      <c r="B7" s="37">
+        <v>15730</v>
+      </c>
+      <c r="C7" s="39">
+        <v>3.1453457680802391E-2</v>
+      </c>
+      <c r="D7" s="37">
+        <v>484466</v>
+      </c>
+      <c r="E7" s="39">
+        <v>0.96873050405515648</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="37">
+        <v>6</v>
+      </c>
+      <c r="B8" s="37">
+        <v>7833</v>
+      </c>
+      <c r="C8" s="39">
+        <v>1.5662742149632876E-2</v>
+      </c>
+      <c r="D8" s="37">
+        <v>492299</v>
+      </c>
+      <c r="E8" s="39">
+        <v>0.98439324620478941</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="37">
+        <v>7</v>
+      </c>
+      <c r="B9" s="37">
+        <v>3970</v>
+      </c>
+      <c r="C9" s="39">
+        <v>7.9383488234447235E-3</v>
+      </c>
+      <c r="D9" s="37">
+        <v>496269</v>
+      </c>
+      <c r="E9" s="39">
+        <v>0.99233159502823409</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="37">
+        <v>8</v>
+      </c>
+      <c r="B10" s="37">
+        <v>1953</v>
+      </c>
+      <c r="C10" s="39">
+        <v>3.9051877209540418E-3</v>
+      </c>
+      <c r="D10" s="37">
+        <v>498222</v>
+      </c>
+      <c r="E10" s="39">
+        <v>0.99623678274918814</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="37">
+        <v>9</v>
+      </c>
+      <c r="B11" s="37">
+        <v>897</v>
+      </c>
+      <c r="C11" s="39">
+        <v>1.7936269255994753E-3</v>
+      </c>
+      <c r="D11" s="37">
+        <v>499119</v>
+      </c>
+      <c r="E11" s="39">
+        <v>0.99803040967478762</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="37">
+        <v>10</v>
+      </c>
+      <c r="B12" s="37">
+        <v>489</v>
+      </c>
+      <c r="C12" s="39">
+        <v>9.7779661830339282E-4</v>
+      </c>
+      <c r="D12" s="37">
+        <v>499608</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.99900820629309106</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="37">
+        <v>11</v>
+      </c>
+      <c r="B13" s="37">
+        <v>246</v>
+      </c>
+      <c r="C13" s="39">
+        <v>4.918976852814615E-4</v>
+      </c>
+      <c r="D13" s="37">
+        <v>499854</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.99950010397837252</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="37">
+        <v>12</v>
+      </c>
+      <c r="B14" s="37">
+        <v>122</v>
+      </c>
+      <c r="C14" s="39">
+        <v>2.4394925855422071E-4</v>
+      </c>
+      <c r="D14" s="37">
+        <v>499976</v>
+      </c>
+      <c r="E14" s="39">
+        <v>0.99974405323692672</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="37">
+        <v>13</v>
+      </c>
+      <c r="B15" s="37">
+        <v>65</v>
+      </c>
+      <c r="C15" s="39">
+        <v>1.2997296562315038E-4</v>
+      </c>
+      <c r="D15" s="37">
+        <v>500041</v>
+      </c>
+      <c r="E15" s="39">
+        <v>0.99987402620254984</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="37">
+        <v>14</v>
+      </c>
+      <c r="B16" s="37">
+        <v>31</v>
+      </c>
+      <c r="C16" s="39">
+        <v>6.1987106681810183E-5</v>
+      </c>
+      <c r="D16" s="37">
+        <v>500072</v>
+      </c>
+      <c r="E16" s="39">
+        <v>0.99993601330923165</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="37">
+        <v>15</v>
+      </c>
+      <c r="B17" s="37">
+        <v>17</v>
+      </c>
+      <c r="C17" s="39">
+        <v>3.3992929470670104E-5</v>
+      </c>
+      <c r="D17" s="37">
+        <v>500089</v>
+      </c>
+      <c r="E17" s="39">
+        <v>0.99997000623870236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="37">
+        <v>16</v>
+      </c>
+      <c r="B18" s="37">
+        <v>4</v>
+      </c>
+      <c r="C18" s="39">
+        <v>7.9983363460400245E-6</v>
+      </c>
+      <c r="D18" s="37">
+        <v>500093</v>
+      </c>
+      <c r="E18" s="39">
+        <v>0.99997800457504837</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="37">
+        <v>17</v>
+      </c>
+      <c r="B19" s="37">
+        <v>5</v>
+      </c>
+      <c r="C19" s="39">
+        <v>9.9979204325500302E-6</v>
+      </c>
+      <c r="D19" s="37">
+        <v>500098</v>
+      </c>
+      <c r="E19" s="39">
+        <v>0.99998800249548092</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="37">
+        <v>18</v>
+      </c>
+      <c r="B20" s="37">
+        <v>3</v>
+      </c>
+      <c r="C20" s="39">
+        <v>5.9987522595300179E-6</v>
+      </c>
+      <c r="D20" s="37">
+        <v>500101</v>
+      </c>
+      <c r="E20" s="39">
+        <v>0.99999400124774052</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="37">
+        <v>19</v>
+      </c>
+      <c r="B21" s="37">
+        <v>3</v>
+      </c>
+      <c r="C21" s="39">
+        <v>5.9987522595300179E-6</v>
+      </c>
+      <c r="D21" s="37">
+        <v>500104</v>
+      </c>
+      <c r="E21" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="37">
+        <v>20</v>
+      </c>
+      <c r="B22" s="37">
+        <v>0</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="37">
+        <v>21</v>
+      </c>
+      <c r="B23" s="37">
+        <v>0</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="37">
+        <v>22</v>
+      </c>
+      <c r="B24" s="37">
+        <v>0</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="37">
+        <v>23</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="37">
+        <v>24</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="37">
+        <v>25</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="37">
+        <v>26</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="37">
+        <v>27</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>